<commit_message>
sm5mini: fixbug upgrade will fail
Change-Id: Ib92f5ce93bdd4c5581eacf3ddff6ba94d7a79612

Former-commit-id: b61f9648c69f64340e191d96285d4594b68a1f56
</commit_message>
<xml_diff>
--- a/SM5MINI/config.xlsx
+++ b/SM5MINI/config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowHeight="18255" tabRatio="500"/>
+    <workbookView windowHeight="17415" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="pin" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="169">
   <si>
     <t>Pin number</t>
   </si>
@@ -532,9 +532,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
     <numFmt numFmtId="176" formatCode="0.0"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="23">
@@ -551,45 +551,14 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
+      <sz val="10"/>
+      <name val="Arial"/>
       <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -604,6 +573,14 @@
     </font>
     <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -611,9 +588,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -637,12 +621,21 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -651,7 +644,15 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -669,8 +670,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -683,25 +699,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -734,43 +734,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -782,139 +914,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -947,32 +947,6 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -1017,15 +991,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1040,141 +1005,176 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="34" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="35" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="32" borderId="9" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="7" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="34" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="8" borderId="6" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="6" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="5" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="4" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="4" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="22" fillId="35" borderId="9" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1600,8 +1600,8 @@
   <sheetPr/>
   <dimension ref="A1:J37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
@@ -1786,18 +1786,12 @@
       <c r="D6" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="6">
-        <v>0</v>
-      </c>
+      <c r="E6" s="6"/>
       <c r="F6" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="G6" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>15</v>
-      </c>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
       <c r="I6" s="6"/>
       <c r="J6" s="15" t="s">
         <v>32</v>
@@ -1816,18 +1810,12 @@
       <c r="D7" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="6">
-        <v>0</v>
-      </c>
+      <c r="E7" s="6"/>
       <c r="F7" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="G7" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>15</v>
-      </c>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
       <c r="I7" s="6"/>
       <c r="J7" s="15" t="s">
         <v>36</v>

</xml_diff>

<commit_message>
sm5 mini update version table
Change-Id: I45d739a52c989cbf741afa3355a74ded580b5306

Former-commit-id: 25c5d58e82f19b7f1b8dbea0db583acb1016a220
</commit_message>
<xml_diff>
--- a/SM5MINI/config.xlsx
+++ b/SM5MINI/config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowHeight="17415" tabRatio="500"/>
+    <workbookView windowHeight="17415" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="pin" sheetId="1" r:id="rId1"/>
@@ -533,9 +533,9 @@
   <numFmts count="5">
     <numFmt numFmtId="176" formatCode="0.0"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -551,53 +551,21 @@
       <charset val="1"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <charset val="134"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -612,9 +580,31 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -633,6 +623,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
@@ -641,8 +646,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -657,36 +670,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -699,13 +691,21 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="36">
     <fill>
@@ -734,73 +734,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -812,67 +902,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -884,37 +914,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -947,15 +947,6 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
@@ -972,6 +963,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1006,6 +1006,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -1025,156 +1040,141 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="34" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="6" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="5" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="3" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="3" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="6" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="5" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="4" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="4" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="22" fillId="35" borderId="9" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="7" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1600,7 +1600,7 @@
   <sheetPr/>
   <dimension ref="A1:J37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" topLeftCell="C1" workbookViewId="0">
+    <sheetView zoomScale="200" zoomScaleNormal="200" topLeftCell="C1" workbookViewId="0">
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
@@ -2903,14 +2903,17 @@
   <sheetPr/>
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelRow="6" outlineLevelCol="5"/>
   <cols>
     <col min="1" max="1" width="14.7733333333333" customWidth="true"/>
-    <col min="2" max="1023" width="8.67333333333333" customWidth="true"/>
+    <col min="2" max="2" width="8.67333333333333" customWidth="true"/>
+    <col min="3" max="3" width="7.3" customWidth="true"/>
+    <col min="4" max="5" width="12.5" customWidth="true"/>
+    <col min="6" max="1023" width="8.67333333333333" customWidth="true"/>
     <col min="1024" max="1025" width="11.52"/>
   </cols>
   <sheetData>
@@ -2945,14 +2948,14 @@
         <v>0</v>
       </c>
       <c r="D2" s="2">
-        <f t="shared" ref="D2:D7" si="0">1.8*C2/(C2+B2)</f>
+        <f>1.8*C2/(C2+B2)</f>
         <v>0</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <f t="shared" ref="F2:F7" si="1">INT(E2/1.8*2^12)</f>
+        <f>INT(E2/1.8*2^12)</f>
         <v>0</v>
       </c>
     </row>
@@ -2967,7 +2970,7 @@
         <v>1000</v>
       </c>
       <c r="D3" s="2">
-        <f t="shared" si="0"/>
+        <f>1.8*C3/(C3+B3)</f>
         <v>0.163636363636364</v>
       </c>
       <c r="E3">
@@ -2975,7 +2978,7 @@
         <v>0.0818181818181818</v>
       </c>
       <c r="F3">
-        <f t="shared" si="1"/>
+        <f>INT(E3/1.8*2^12)</f>
         <v>186</v>
       </c>
     </row>
@@ -2987,19 +2990,19 @@
         <v>10000</v>
       </c>
       <c r="C4" s="2">
-        <v>3000</v>
+        <v>4700</v>
       </c>
       <c r="D4" s="2">
-        <f t="shared" si="0"/>
-        <v>0.415384615384615</v>
+        <f>1.8*C4/(C4+B4)</f>
+        <v>0.575510204081633</v>
       </c>
       <c r="E4">
         <f>D4-(D4-D3)/2</f>
-        <v>0.28951048951049</v>
+        <v>0.369573283858998</v>
       </c>
       <c r="F4">
-        <f t="shared" si="1"/>
-        <v>658</v>
+        <f>INT(E4/1.8*2^12)</f>
+        <v>840</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -3010,19 +3013,19 @@
         <v>10000</v>
       </c>
       <c r="C5" s="2">
-        <v>5600</v>
+        <v>10000</v>
       </c>
       <c r="D5" s="2">
-        <f t="shared" si="0"/>
-        <v>0.646153846153846</v>
+        <f>1.8*C5/(C5+B5)</f>
+        <v>0.9</v>
       </c>
       <c r="E5">
         <f>D5-(D5-D4)/2</f>
-        <v>0.530769230769231</v>
+        <v>0.737755102040816</v>
       </c>
       <c r="F5">
-        <f t="shared" si="1"/>
-        <v>1207</v>
+        <f>INT(E5/1.8*2^12)</f>
+        <v>1678</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -3033,19 +3036,19 @@
         <v>10000</v>
       </c>
       <c r="C6" s="2">
-        <v>10000</v>
+        <v>47000</v>
       </c>
       <c r="D6" s="2">
-        <f t="shared" si="0"/>
-        <v>0.9</v>
+        <f>1.8*C6/(C6+B6)</f>
+        <v>1.48421052631579</v>
       </c>
       <c r="E6">
         <f>D6-(D6-D5)/2</f>
-        <v>0.773076923076923</v>
+        <v>1.19210526315789</v>
       </c>
       <c r="F6">
-        <f t="shared" si="1"/>
-        <v>1759</v>
+        <f>INT(E6/1.8*2^12)</f>
+        <v>2712</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -3055,20 +3058,20 @@
       <c r="B7" s="2">
         <v>10000</v>
       </c>
-      <c r="C7" s="2">
-        <v>18000</v>
+      <c r="C7">
+        <v>100000</v>
       </c>
       <c r="D7" s="2">
-        <f t="shared" si="0"/>
-        <v>1.15714285714286</v>
+        <f>1.8*C7/(C7+B7)</f>
+        <v>1.63636363636364</v>
       </c>
       <c r="E7">
         <f>D7-(D7-D6)/2</f>
-        <v>1.02857142857143</v>
+        <v>1.56028708133971</v>
       </c>
       <c r="F7">
-        <f t="shared" si="1"/>
-        <v>2340</v>
+        <f>INT(E7/1.8*2^12)</f>
+        <v>3550</v>
       </c>
     </row>
   </sheetData>

</xml_diff>